<commit_message>
Adding labs with a correct ic
</commit_message>
<xml_diff>
--- a/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
+++ b/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H18"/>
     </sheetView>
   </sheetViews>
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>1600</v>
+        <v>1596</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -599,25 +599,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" s="4">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="D6" s="4">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="E6" s="4">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="F6" s="4">
-        <v>341</v>
+        <v>374</v>
       </c>
       <c r="G6" s="4">
-        <v>430</v>
+        <v>481</v>
       </c>
       <c r="H6" s="4">
-        <v>323</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="60.75" thickBot="1">
@@ -625,25 +625,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C7" s="4">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D7" s="4">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E7" s="4">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F7" s="4">
+        <v>99</v>
+      </c>
+      <c r="G7" s="4">
+        <v>116</v>
+      </c>
+      <c r="H7" s="4">
         <v>95</v>
-      </c>
-      <c r="G7" s="4">
-        <v>110</v>
-      </c>
-      <c r="H7" s="4">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60.75" thickBot="1">
@@ -651,25 +651,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>55.1</v>
+        <v>56.2</v>
       </c>
       <c r="C8" s="4">
-        <v>17.600000000000001</v>
+        <v>16.7</v>
       </c>
       <c r="D8" s="4">
-        <v>18.7</v>
+        <v>17.8</v>
       </c>
       <c r="E8" s="4">
-        <v>19.8</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F8" s="4">
-        <v>20.9</v>
+        <v>20.3</v>
       </c>
       <c r="G8" s="4">
-        <v>23.5</v>
+        <v>23.2</v>
       </c>
       <c r="H8" s="4">
-        <v>20.3</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75.75" thickBot="1">
@@ -677,25 +677,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="C9" s="4">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D9" s="4">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="E9" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="H9" s="4">
         <v>1.7</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="G9" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60.75" thickBot="1">
@@ -706,22 +706,22 @@
         <v>7.6</v>
       </c>
       <c r="C10" s="4">
-        <v>19.600000000000001</v>
+        <v>20.6</v>
       </c>
       <c r="D10" s="4">
-        <v>21.2</v>
+        <v>22.4</v>
       </c>
       <c r="E10" s="4">
-        <v>22.8</v>
+        <v>24.3</v>
       </c>
       <c r="F10" s="4">
-        <v>24.4</v>
+        <v>26.1</v>
       </c>
       <c r="G10" s="4">
-        <v>28.2</v>
+        <v>30.3</v>
       </c>
       <c r="H10" s="4">
-        <v>39.799999999999997</v>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45.75" thickBot="1">
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>24</v>
@@ -741,13 +741,13 @@
         <v>24</v>
       </c>
       <c r="F11" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="4">
         <v>25</v>
       </c>
       <c r="H11" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60.75" thickBot="1">
@@ -755,25 +755,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C12" s="4">
         <v>103</v>
       </c>
       <c r="D12" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="4">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" s="4">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" s="4">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H12" s="4">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60.75" thickBot="1">
@@ -781,25 +781,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>13.3</v>
+        <v>12.5</v>
       </c>
       <c r="C13" s="4">
-        <v>34.1</v>
+        <v>33.9</v>
       </c>
       <c r="D13" s="4">
-        <v>33.4</v>
+        <v>33.1</v>
       </c>
       <c r="E13" s="4">
-        <v>32.6</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="F13" s="4">
-        <v>31.8</v>
+        <v>31.4</v>
       </c>
       <c r="G13" s="4">
-        <v>30</v>
+        <v>29.4</v>
       </c>
       <c r="H13" s="4">
-        <v>53.3</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45.75" thickBot="1">
@@ -807,25 +807,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C14" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="4">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G14" s="4">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="H14" s="4">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75.75" thickBot="1">
@@ -833,25 +833,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" s="4">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H15" s="4">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45.75" thickBot="1">
@@ -862,22 +862,22 @@
         <v>100</v>
       </c>
       <c r="C16" s="4">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4">
         <v>59</v>
       </c>
-      <c r="D16" s="4">
-        <v>58</v>
-      </c>
-      <c r="E16" s="4">
-        <v>58</v>
-      </c>
       <c r="F16" s="4">
+        <v>59</v>
+      </c>
+      <c r="G16" s="4">
         <v>57</v>
       </c>
-      <c r="G16" s="4">
-        <v>56</v>
-      </c>
       <c r="H16" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45.75" thickBot="1">
@@ -885,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>19.8</v>
+        <v>20.6</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -911,25 +911,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4">
+        <v>348</v>
+      </c>
+      <c r="D18" s="4">
+        <v>343</v>
+      </c>
+      <c r="E18" s="4">
+        <v>328</v>
+      </c>
+      <c r="F18" s="4">
         <v>311</v>
       </c>
-      <c r="D18" s="4">
-        <v>307</v>
-      </c>
-      <c r="E18" s="4">
-        <v>295</v>
-      </c>
-      <c r="F18" s="4">
-        <v>280</v>
-      </c>
       <c r="G18" s="4">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="H18" s="4">
-        <v>297</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding HumMod data to Lab 16
</commit_message>
<xml_diff>
--- a/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
+++ b/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Diabetes Mellitus Meal Data</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Plasma [Gluca’n](pg/mL)</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>For HumMod data, using the button that stops all insulin secretion added in my modified files.</t>
+  </si>
+  <si>
+    <t>Fat triglyceride uptake not a variable in HumMod, using hydrolysis instead.</t>
   </si>
 </sst>
 </file>
@@ -97,12 +109,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -169,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -182,6 +200,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,20 +504,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,8 +556,32 @@
       <c r="H2" s="2">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="60.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -541,8 +606,32 @@
       <c r="H3" s="4">
         <v>13923</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1903.9</v>
+      </c>
+      <c r="M3" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="N3" s="4">
+        <v>19201</v>
+      </c>
+      <c r="O3" s="4">
+        <v>37521.9</v>
+      </c>
+      <c r="P3" s="4">
+        <v>55882</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>37882</v>
+      </c>
+      <c r="R3" s="4">
+        <v>2910.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -567,8 +656,32 @@
       <c r="H4" s="4">
         <v>1271</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1963.5</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>8250.6</v>
+      </c>
+      <c r="O4" s="4">
+        <v>14366.3</v>
+      </c>
+      <c r="P4" s="4">
+        <v>18901.7</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>7668</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1258.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -593,8 +706,32 @@
       <c r="H5" s="4">
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1574.2</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>10060.299999999999</v>
+      </c>
+      <c r="O5" s="4">
+        <v>16153.8</v>
+      </c>
+      <c r="P5" s="4">
+        <v>19850.099999999999</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>4402.2</v>
+      </c>
+      <c r="R5" s="4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -619,8 +756,32 @@
       <c r="H6" s="4">
         <v>251</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4">
+        <v>100.7</v>
+      </c>
+      <c r="M6" s="4">
+        <v>208.9</v>
+      </c>
+      <c r="N6" s="4">
+        <v>237.5</v>
+      </c>
+      <c r="O6" s="4">
+        <v>268.89999999999998</v>
+      </c>
+      <c r="P6" s="4">
+        <v>297.60000000000002</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>366.7</v>
+      </c>
+      <c r="R6" s="4">
+        <v>418.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="60.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -645,8 +806,32 @@
       <c r="H7" s="4">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="M7" s="4">
+        <v>60.3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>62.3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="P7" s="4">
+        <v>65.7</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>65.5</v>
+      </c>
+      <c r="R7" s="4">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -671,8 +856,32 @@
       <c r="H8" s="4">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="75.75" thickBot="1">
+      <c r="K8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="4">
+        <v>47.7</v>
+      </c>
+      <c r="M8" s="4">
+        <v>26.2</v>
+      </c>
+      <c r="N8" s="4">
+        <v>27.4</v>
+      </c>
+      <c r="O8" s="4">
+        <v>28.5</v>
+      </c>
+      <c r="P8" s="4">
+        <v>29.1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>29.7</v>
+      </c>
+      <c r="R8" s="4">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="75.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -697,8 +906,32 @@
       <c r="H9" s="4">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="P9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="60.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -723,8 +956,32 @@
       <c r="H10" s="4">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="M10" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="N10" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="O10" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="P10" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="R10" s="4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="45.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -749,8 +1006,32 @@
       <c r="H11" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>28.2</v>
+      </c>
+      <c r="N11" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="O11" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="P11" s="4">
+        <v>30.5</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="R11" s="4">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="60.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -775,8 +1056,32 @@
       <c r="H12" s="4">
         <v>135</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="4">
+        <v>82.4</v>
+      </c>
+      <c r="M12" s="4">
+        <v>77.3</v>
+      </c>
+      <c r="N12" s="4">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="O12" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="P12" s="4">
+        <v>73.3</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="R12" s="4">
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="60.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -801,8 +1106,32 @@
       <c r="H13" s="4">
         <v>56.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="4">
+        <v>14.9</v>
+      </c>
+      <c r="M13" s="4">
+        <v>14.4</v>
+      </c>
+      <c r="N13" s="4">
+        <v>13.9</v>
+      </c>
+      <c r="O13" s="4">
+        <v>13.3</v>
+      </c>
+      <c r="P13" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>12.6</v>
+      </c>
+      <c r="R13" s="4">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="45.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -827,8 +1156,32 @@
       <c r="H14" s="4">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="75.75" thickBot="1">
+      <c r="K14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="4">
+        <v>101.1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="N14" s="4">
+        <v>42.6</v>
+      </c>
+      <c r="O14" s="4">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="P14" s="4">
+        <v>99</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>142</v>
+      </c>
+      <c r="R14" s="4">
+        <v>110.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="75.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -853,8 +1206,32 @@
       <c r="H15" s="4">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4">
+        <v>103.2</v>
+      </c>
+      <c r="M15" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="N15" s="4">
+        <v>7.7</v>
+      </c>
+      <c r="O15" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="P15" s="4">
+        <v>97</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>218.6</v>
+      </c>
+      <c r="R15" s="4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="45.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -879,8 +1256,32 @@
       <c r="H16" s="4">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="45.75" thickBot="1">
+      <c r="K16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="4">
+        <v>113.7</v>
+      </c>
+      <c r="M16" s="4">
+        <v>62.1</v>
+      </c>
+      <c r="N16" s="4">
+        <v>61.4</v>
+      </c>
+      <c r="O16" s="4">
+        <v>60.8</v>
+      </c>
+      <c r="P16" s="4">
+        <v>60.3</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>58.6</v>
+      </c>
+      <c r="R16" s="4">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="45.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -905,8 +1306,32 @@
       <c r="H17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="60.75" thickBot="1">
+      <c r="K17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="4">
+        <v>20.8</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="60.75" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -931,8 +1356,70 @@
       <c r="H18" s="4">
         <v>400</v>
       </c>
+      <c r="K18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="4">
+        <v>68.8</v>
+      </c>
+      <c r="M18" s="4">
+        <v>337.4</v>
+      </c>
+      <c r="N18" s="4">
+        <v>333</v>
+      </c>
+      <c r="O18" s="4">
+        <v>320.3</v>
+      </c>
+      <c r="P18" s="4">
+        <v>303.8</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>259.10000000000002</v>
+      </c>
+      <c r="R18" s="4">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="K20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="K23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K20:R21"/>
+    <mergeCell ref="K23:R23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding percentage data to Lab 16
</commit_message>
<xml_diff>
--- a/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
+++ b/16_diabetes_mellitus/16_diabetes_mellitus_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>Diabetes Mellitus Meal Data</t>
   </si>
@@ -82,13 +82,19 @@
   </si>
   <si>
     <t>Fat triglyceride uptake not a variable in HumMod, using hydrolysis instead.</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +113,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -184,10 +197,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -210,11 +224,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -504,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,7 +567,7 @@
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,8 +580,14 @@
       <c r="O1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,8 +636,32 @@
       <c r="R2" s="2">
         <v>0.375</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0.375</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="60.75" thickBot="1">
+    <row r="3" spans="1:28" ht="60.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -630,8 +710,38 @@
       <c r="R3" s="4">
         <v>2910.1</v>
       </c>
+      <c r="U3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="8">
+        <f>ABS((B3-L3)/B3)</f>
+        <v>1.3523316062176119E-2</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="8">
+        <f t="shared" ref="X3:X18" si="0">ABS((D3-N3)/D3)</f>
+        <v>4.4298442088497335E-2</v>
+      </c>
+      <c r="Y3" s="8">
+        <f t="shared" ref="Y3:Y18" si="1">ABS((E3-O3)/E3)</f>
+        <v>4.9621336845571254E-2</v>
+      </c>
+      <c r="Z3" s="8">
+        <f t="shared" ref="Z3:Z18" si="2">ABS((F3-P3)/F3)</f>
+        <v>5.0772026974231797E-2</v>
+      </c>
+      <c r="AA3" s="8">
+        <f t="shared" ref="AA3:AA18" si="3">ABS((G3-Q3)/G3)</f>
+        <v>0.1375361427953464</v>
+      </c>
+      <c r="AB3" s="8">
+        <f t="shared" ref="AB3:AB18" si="4">ABS((H3-R3)/H3)</f>
+        <v>0.79098613804496154</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" ht="45.75" thickBot="1">
+    <row r="4" spans="1:28" ht="45.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -680,8 +790,38 @@
       <c r="R4" s="4">
         <v>1258.7</v>
       </c>
+      <c r="U4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="8">
+        <f t="shared" ref="V4:V18" si="5">ABS((B4-L4)/B4)</f>
+        <v>1.3812154696132596E-2</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7509991522340272E-4</v>
+      </c>
+      <c r="Y4" s="8">
+        <f t="shared" si="1"/>
+        <v>6.0521739130439841E-4</v>
+      </c>
+      <c r="Z4" s="8">
+        <f t="shared" si="2"/>
+        <v>2.8031945840161171E-4</v>
+      </c>
+      <c r="AA4" s="8">
+        <f t="shared" si="3"/>
+        <v>2.4717054767789777E-3</v>
+      </c>
+      <c r="AB4" s="8">
+        <f t="shared" si="4"/>
+        <v>9.6774193548386737E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="45.75" thickBot="1">
+    <row r="5" spans="1:28" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -730,8 +870,38 @@
       <c r="R5" s="4">
         <v>215</v>
       </c>
+      <c r="U5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="8">
+        <f t="shared" si="5"/>
+        <v>1.3659147869674157E-2</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0248756218904748E-3</v>
+      </c>
+      <c r="Y5" s="8">
+        <f t="shared" si="1"/>
+        <v>4.8309178743956847E-4</v>
+      </c>
+      <c r="Z5" s="8">
+        <f t="shared" si="2"/>
+        <v>3.578087990726475E-4</v>
+      </c>
+      <c r="AA5" s="8">
+        <f t="shared" si="3"/>
+        <v>5.8265582655826972E-3</v>
+      </c>
+      <c r="AB5" s="8">
+        <f t="shared" si="4"/>
+        <v>2.2727272727272728E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="45.75" thickBot="1">
+    <row r="6" spans="1:28" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -780,8 +950,39 @@
       <c r="R6" s="4">
         <v>418.5</v>
       </c>
+      <c r="U6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="8">
+        <f t="shared" si="5"/>
+        <v>5.8878504672897167E-2</v>
+      </c>
+      <c r="W6" s="8">
+        <f t="shared" ref="W3:W18" si="6">ABS((C6-M6)/C6)</f>
+        <v>0.22629629629629627</v>
+      </c>
+      <c r="X6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.21096345514950166</v>
+      </c>
+      <c r="Y6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.20443786982248527</v>
+      </c>
+      <c r="Z6" s="8">
+        <f t="shared" si="2"/>
+        <v>0.20427807486631011</v>
+      </c>
+      <c r="AA6" s="8">
+        <f t="shared" si="3"/>
+        <v>0.23762993762993764</v>
+      </c>
+      <c r="AB6" s="8">
+        <f t="shared" si="4"/>
+        <v>0.66733067729083662</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="60.75" thickBot="1">
+    <row r="7" spans="1:28" ht="60.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -830,8 +1031,39 @@
       <c r="R7" s="4">
         <v>78.5</v>
       </c>
+      <c r="U7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="8">
+        <f t="shared" si="5"/>
+        <v>0.25566037735849051</v>
+      </c>
+      <c r="W7" s="8">
+        <f t="shared" si="6"/>
+        <v>0.23670886075949371</v>
+      </c>
+      <c r="X7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.27558139534883724</v>
+      </c>
+      <c r="Y7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.30322580645161296</v>
+      </c>
+      <c r="Z7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.33636363636363631</v>
+      </c>
+      <c r="AA7" s="8">
+        <f t="shared" si="3"/>
+        <v>0.43534482758620691</v>
+      </c>
+      <c r="AB7" s="8">
+        <f t="shared" si="4"/>
+        <v>0.1736842105263158</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" ht="60.75" thickBot="1">
+    <row r="8" spans="1:28" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -880,8 +1112,39 @@
       <c r="R8" s="4">
         <v>31.1</v>
       </c>
+      <c r="U8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="5"/>
+        <v>0.15124555160142347</v>
+      </c>
+      <c r="W8" s="8">
+        <f t="shared" si="6"/>
+        <v>0.56886227544910184</v>
+      </c>
+      <c r="X8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.53932584269662909</v>
+      </c>
+      <c r="Y8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.49214659685863865</v>
+      </c>
+      <c r="Z8" s="8">
+        <f t="shared" si="2"/>
+        <v>0.43349753694581283</v>
+      </c>
+      <c r="AA8" s="8">
+        <f t="shared" si="3"/>
+        <v>0.28017241379310348</v>
+      </c>
+      <c r="AB8" s="8">
+        <f t="shared" si="4"/>
+        <v>1.0326797385620916</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" ht="75.75" thickBot="1">
+    <row r="9" spans="1:28" ht="75.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -930,8 +1193,39 @@
       <c r="R9" s="4">
         <v>1.7</v>
       </c>
+      <c r="U9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="5"/>
+        <v>0.18750000000000003</v>
+      </c>
+      <c r="W9" s="8">
+        <f t="shared" si="6"/>
+        <v>0.18750000000000003</v>
+      </c>
+      <c r="X9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222229</v>
+      </c>
+      <c r="Y9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.21052631578947364</v>
+      </c>
+      <c r="Z9" s="8">
+        <f t="shared" si="2"/>
+        <v>0.28571428571428575</v>
+      </c>
+      <c r="AA9" s="8">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="AB9" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" ht="60.75" thickBot="1">
+    <row r="10" spans="1:28" ht="60.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -980,8 +1274,39 @@
       <c r="R10" s="4">
         <v>8.9</v>
       </c>
+      <c r="U10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="8">
+        <f t="shared" si="5"/>
+        <v>0.22368421052631571</v>
+      </c>
+      <c r="W10" s="8">
+        <f t="shared" si="6"/>
+        <v>0.69417475728155342</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.6919642857142857</v>
+      </c>
+      <c r="Y10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.69547325102880653</v>
+      </c>
+      <c r="Z10" s="8">
+        <f t="shared" si="2"/>
+        <v>0.71264367816091956</v>
+      </c>
+      <c r="AA10" s="8">
+        <f t="shared" si="3"/>
+        <v>0.77557755775577553</v>
+      </c>
+      <c r="AB10" s="8">
+        <f t="shared" si="4"/>
+        <v>0.73273273273273276</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" ht="45.75" thickBot="1">
+    <row r="11" spans="1:28" ht="45.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1030,8 +1355,39 @@
       <c r="R11" s="4">
         <v>36.299999999999997</v>
       </c>
+      <c r="U11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="8">
+        <f t="shared" si="5"/>
+        <v>0.51</v>
+      </c>
+      <c r="W11" s="8">
+        <f t="shared" si="6"/>
+        <v>0.17499999999999996</v>
+      </c>
+      <c r="X11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.17083333333333339</v>
+      </c>
+      <c r="Y11" s="8">
+        <f t="shared" si="1"/>
+        <v>0.19166666666666674</v>
+      </c>
+      <c r="Z11" s="8">
+        <f t="shared" si="2"/>
+        <v>0.22</v>
+      </c>
+      <c r="AA11" s="8">
+        <f t="shared" si="3"/>
+        <v>0.61199999999999988</v>
+      </c>
+      <c r="AB11" s="8">
+        <f t="shared" si="4"/>
+        <v>0.57826086956521727</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" ht="60.75" thickBot="1">
+    <row r="12" spans="1:28" ht="60.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1080,8 +1436,39 @@
       <c r="R12" s="4">
         <v>70.2</v>
       </c>
+      <c r="U12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="8">
+        <f t="shared" si="5"/>
+        <v>7.2289156626505341E-3</v>
+      </c>
+      <c r="W12" s="8">
+        <f t="shared" si="6"/>
+        <v>0.24951456310679615</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.23900000000000005</v>
+      </c>
+      <c r="Y12" s="8">
+        <f t="shared" si="1"/>
+        <v>0.24081632653061219</v>
+      </c>
+      <c r="Z12" s="8">
+        <f t="shared" si="2"/>
+        <v>0.22842105263157897</v>
+      </c>
+      <c r="AA12" s="8">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000008</v>
+      </c>
+      <c r="AB12" s="8">
+        <f t="shared" si="4"/>
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" ht="60.75" thickBot="1">
+    <row r="13" spans="1:28" ht="60.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1130,8 +1517,39 @@
       <c r="R13" s="4">
         <v>13.1</v>
       </c>
+      <c r="U13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="8">
+        <f t="shared" si="5"/>
+        <v>0.19200000000000003</v>
+      </c>
+      <c r="W13" s="8">
+        <f t="shared" si="6"/>
+        <v>0.5752212389380531</v>
+      </c>
+      <c r="X13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58006042296072513</v>
+      </c>
+      <c r="Y13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.58695652173913049</v>
+      </c>
+      <c r="Z13" s="8">
+        <f t="shared" si="2"/>
+        <v>0.5859872611464968</v>
+      </c>
+      <c r="AA13" s="8">
+        <f t="shared" si="3"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AB13" s="8">
+        <f t="shared" si="4"/>
+        <v>0.768141592920354</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" ht="45.75" thickBot="1">
+    <row r="14" spans="1:28" ht="45.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1180,8 +1598,39 @@
       <c r="R14" s="4">
         <v>110.7</v>
       </c>
+      <c r="U14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" s="8">
+        <f t="shared" si="5"/>
+        <v>0.12333333333333327</v>
+      </c>
+      <c r="W14" s="8">
+        <f t="shared" si="6"/>
+        <v>1.2533333333333332</v>
+      </c>
+      <c r="X14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Y14" s="8">
+        <f t="shared" si="1"/>
+        <v>0.35510204081632663</v>
+      </c>
+      <c r="Z14" s="8">
+        <f t="shared" si="2"/>
+        <v>0.17857142857142858</v>
+      </c>
+      <c r="AA14" s="8">
+        <f t="shared" si="3"/>
+        <v>7.1895424836601302E-2</v>
+      </c>
+      <c r="AB14" s="8">
+        <f t="shared" si="4"/>
+        <v>0.31242236024844716</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" ht="75.75" thickBot="1">
+    <row r="15" spans="1:28" ht="75.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1230,8 +1679,39 @@
       <c r="R15" s="4">
         <v>132</v>
       </c>
+      <c r="U15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V15" s="8">
+        <f t="shared" si="5"/>
+        <v>0.12173913043478264</v>
+      </c>
+      <c r="W15" s="8">
+        <f t="shared" si="6"/>
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="X15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="Y15" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22083333333333335</v>
+      </c>
+      <c r="Z15" s="8">
+        <f t="shared" si="2"/>
+        <v>1.3095238095238095</v>
+      </c>
+      <c r="AA15" s="8">
+        <f t="shared" si="3"/>
+        <v>1.8763157894736842</v>
+      </c>
+      <c r="AB15" s="8">
+        <f t="shared" si="4"/>
+        <v>0.62962962962962965</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" ht="45.75" thickBot="1">
+    <row r="16" spans="1:28" ht="45.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1280,8 +1760,39 @@
       <c r="R16" s="4">
         <v>53.2</v>
       </c>
+      <c r="U16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" s="8">
+        <f t="shared" si="5"/>
+        <v>0.13700000000000004</v>
+      </c>
+      <c r="W16" s="8">
+        <f t="shared" si="6"/>
+        <v>3.5000000000000024E-2</v>
+      </c>
+      <c r="X16" s="8">
+        <f t="shared" si="0"/>
+        <v>2.333333333333331E-2</v>
+      </c>
+      <c r="Y16" s="8">
+        <f t="shared" si="1"/>
+        <v>3.0508474576271139E-2</v>
+      </c>
+      <c r="Z16" s="8">
+        <f t="shared" si="2"/>
+        <v>2.2033898305084697E-2</v>
+      </c>
+      <c r="AA16" s="8">
+        <f t="shared" si="3"/>
+        <v>2.8070175438596516E-2</v>
+      </c>
+      <c r="AB16" s="8">
+        <f t="shared" si="4"/>
+        <v>4.3137254901960839E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" ht="45.75" thickBot="1">
+    <row r="17" spans="1:28" ht="45.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1330,8 +1841,33 @@
       <c r="R17" s="4">
         <v>0</v>
       </c>
+      <c r="U17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V17" s="8">
+        <f t="shared" si="5"/>
+        <v>9.7087378640776344E-3</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" ht="60.75" thickBot="1">
+    <row r="18" spans="1:28" ht="60.75" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1380,8 +1916,39 @@
       <c r="R18" s="4">
         <v>243</v>
       </c>
+      <c r="U18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V18" s="8">
+        <f t="shared" si="5"/>
+        <v>0.10649350649350653</v>
+      </c>
+      <c r="W18" s="8">
+        <f t="shared" si="6"/>
+        <v>3.0459770114942594E-2</v>
+      </c>
+      <c r="X18" s="8">
+        <f t="shared" si="0"/>
+        <v>2.9154518950437316E-2</v>
+      </c>
+      <c r="Y18" s="8">
+        <f t="shared" si="1"/>
+        <v>2.3475609756097526E-2</v>
+      </c>
+      <c r="Z18" s="8">
+        <f t="shared" si="2"/>
+        <v>2.3151125401929224E-2</v>
+      </c>
+      <c r="AA18" s="8">
+        <f t="shared" si="3"/>
+        <v>8.1205673758865171E-2</v>
+      </c>
+      <c r="AB18" s="8">
+        <f t="shared" si="4"/>
+        <v>0.39250000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:28">
       <c r="K20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1393,7 +1960,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:28">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1403,7 +1970,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:28">
       <c r="K23" s="7" t="s">
         <v>21</v>
       </c>
@@ -1420,6 +1987,15 @@
     <mergeCell ref="K20:R21"/>
     <mergeCell ref="K23:R23"/>
   </mergeCells>
+  <conditionalFormatting sqref="V3:AB18">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>